<commit_message>
Problem 1-(b) solving: fixed leg
</commit_message>
<xml_diff>
--- a/Homework/HW2/calc.xlsx
+++ b/Homework/HW2/calc.xlsx
@@ -372,9 +372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -569,6 +567,7 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2">
         <f>((1 + E4)^E2) / ((1+D4)^D2) -1</f>
         <v>2.1385542168671279E-2</v>

</xml_diff>